<commit_message>
simulations are going well
</commit_message>
<xml_diff>
--- a/Components/Sipariş Listesi2.xlsx
+++ b/Components/Sipariş Listesi2.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Digikey Part No</t>
   </si>
@@ -132,6 +133,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/texas-instruments/LM340SX-12-NOPB/LM340SX-12-NOPBCT-ND/3526960 </t>
+  </si>
+  <si>
+    <t>P.024AUCT-ND</t>
+  </si>
+  <si>
+    <t>RES 0.024 OHM 1% 1W 1206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-8BWFR024V/P.024AUCT-ND/1711691</t>
+  </si>
+  <si>
+    <t>0.74</t>
   </si>
 </sst>
 </file>
@@ -474,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,4 +757,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Simulations and schematic design are completed. Layout design is started.
</commit_message>
<xml_diff>
--- a/Components/Sipariş Listesi2.xlsx
+++ b/Components/Sipariş Listesi2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,9 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>